<commit_message>
Analisas lexico y sintactico completos
jflex y cup
</commit_message>
<xml_diff>
--- a/Gramatica/Libro1.xlsx
+++ b/Gramatica/Libro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\3D Objects\GitHub\OLC1-P1-202000119\Gramatica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E01134-5773-4921-89BB-650A61780EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD604E1-877A-46B3-96AC-ECCBEDB97FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14775" yWindow="540" windowWidth="19320" windowHeight="14400" activeTab="1" xr2:uid="{27CFFC6D-3C5D-4CAC-85D0-DEC13A38AAA2}"/>
+    <workbookView xWindow="1335" yWindow="735" windowWidth="14505" windowHeight="14400" activeTab="1" xr2:uid="{27CFFC6D-3C5D-4CAC-85D0-DEC13A38AAA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="120">
   <si>
     <t>Tabla de tokens</t>
   </si>
@@ -384,6 +384,18 @@
   </si>
   <si>
     <t xml:space="preserve">S_LINE &lt;DEFER&gt;  | S_ASTERISK  &lt;DEFER&gt;  | S_PLUS &lt;DEFER&gt;  |  S_QMARK &lt;DEFER&gt;  | S_DOT &lt;DEFER&gt; </t>
+  </si>
+  <si>
+    <t>FULLRANK S_SEMICOLON</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NUMBER | LETTER | RANGE | SPACE | S_ASTERISK | S_PLUS | S_COLON | S_DOT |S_DOTS | S_SEMICOLON | S_QMARK | S_LA | S_LINE | S_LLC |S_DQUOTES | S_QUOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NUMBER  |  LETTER | RANGE | S_ASTERISK | S_PLUS | S_COLON | S_DOT  |  S_DOTS  | S_SEMICOLON |  S_QMARK  | S_LA  |  S_LINE  |  S_LLC |S_DQUOTES | S_QUOTE S_LA  |  S_LINE  |  S_LLC</t>
+  </si>
+  <si>
+    <t>S_LLC | &lt;CADENAS&gt;</t>
   </si>
 </sst>
 </file>
@@ -997,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56814442-BCEB-455F-8BF0-4AF474A4C165}">
-  <dimension ref="A7:H69"/>
+  <dimension ref="A7:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E47" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,7 +1804,7 @@
         <v>68</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="6:8" x14ac:dyDescent="0.25">
@@ -1825,7 +1837,7 @@
         <v>68</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="6:8" x14ac:dyDescent="0.25">
@@ -1903,6 +1915,182 @@
       </c>
       <c r="H69" s="2" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F75" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F76" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F77" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F78" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F79" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F80" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="81" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F81" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F82" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="83" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F83" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F84" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F85" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="86" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F86" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="87" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F87" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="88" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F88" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F89" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F90" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>